<commit_message>
add test case for optimization
</commit_message>
<xml_diff>
--- a/Results/performance_vs_optPBN.xlsx
+++ b/Results/performance_vs_optPBN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luna/Desktop/Pancreatic cancer/BNMPy/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BE4CEF-9331-444E-98F8-F04E202AD69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5AE9A0-6221-4041-8DE4-7F4120BD898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1520" windowWidth="30220" windowHeight="20060" xr2:uid="{0F2A5497-3F2F-EF46-83BE-1532FE4FE77A}"/>
+    <workbookView xWindow="880" yWindow="840" windowWidth="33420" windowHeight="20060" xr2:uid="{0F2A5497-3F2F-EF46-83BE-1532FE4FE77A}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="157">
   <si>
     <t>*Note: Disc. = Discrete mode, Cont. = Continuous mode, Ext. = Extended model structure, Init. = Initial model tructure</t>
   </si>
@@ -809,24 +809,6 @@
     <t>0.6118, 0.3882</t>
   </si>
   <si>
-    <t>Model 3</t>
-  </si>
-  <si>
-    <t>Model 4</t>
-  </si>
-  <si>
-    <t>Particle swarm algorithm, PSO</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Differential evolution, DE</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>0.6991, 0.3009</t>
   </si>
   <si>
@@ -840,6 +822,42 @@
   </si>
   <si>
     <t>0.604, 0.3960</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>PSO</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>*Note:</t>
+  </si>
+  <si>
+    <t>iter. = iterations, Delta = difference between steady-state distributions and measurement data</t>
+  </si>
+  <si>
+    <t>Model: Trairatphisan2014</t>
+  </si>
+  <si>
+    <t>iter.</t>
+  </si>
+  <si>
+    <t>Not provided</t>
+  </si>
+  <si>
+    <t>0.7039, 0.2961</t>
+  </si>
+  <si>
+    <t>0.5901, 0.4099</t>
+  </si>
+  <si>
+    <t>0.7009, 0.2991</t>
+  </si>
+  <si>
+    <t>0.5948, 0.4052</t>
   </si>
 </sst>
 </file>
@@ -956,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="69">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -1720,27 +1738,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1781,36 +1782,17 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1820,7 +1802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1924,15 +1906,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1943,9 +1919,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2230,45 +2203,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2278,93 +2215,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2376,25 +2272,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2734,10 +2633,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2767,13 +2666,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -2785,7 +2684,7 @@
     </row>
     <row r="7" spans="1:11" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" t="s">
@@ -2793,91 +2692,91 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="154" t="s">
+    <row r="9" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="155" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="154"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="139"/>
     </row>
     <row r="10" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="189"/>
-      <c r="B10" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="166" t="s">
+      <c r="A10" s="164"/>
+      <c r="B10" s="142" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="143" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="166" t="s">
+      <c r="E10" s="143" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="167" t="s">
+      <c r="G10" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="166" t="s">
+      <c r="H10" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="166" t="s">
+      <c r="I10" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="168" t="s">
+      <c r="J10" s="145" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="156" t="s">
+      <c r="A11" s="140" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="169" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="170">
+      <c r="B11" s="146" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="147">
         <v>1.2558968979802399E-4</v>
       </c>
-      <c r="D11" s="171">
+      <c r="D11" s="148">
         <v>0.02</v>
       </c>
-      <c r="E11" s="171">
+      <c r="E11" s="148">
         <v>5</v>
       </c>
-      <c r="F11" s="171">
+      <c r="F11" s="148">
         <v>31.23</v>
       </c>
-      <c r="G11" s="171" t="s">
+      <c r="G11" s="148" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="171">
+      <c r="H11" s="148">
         <v>1.41E-2</v>
       </c>
-      <c r="I11" s="190" t="s">
+      <c r="I11" s="156" t="s">
         <v>139</v>
       </c>
-      <c r="J11" s="172">
-        <v>0.11799999999999999</v>
+      <c r="J11" s="149">
+        <v>1.18E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="146"/>
-      <c r="B12" s="173"/>
-      <c r="C12" s="159">
+      <c r="A12" s="136"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="141">
         <v>1.3409822281216599E-4</v>
       </c>
       <c r="D12" s="10">
@@ -2890,22 +2789,22 @@
         <v>1105.58</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H12" s="10">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I12" s="191" t="s">
-        <v>147</v>
+      <c r="I12" s="157" t="s">
+        <v>141</v>
       </c>
       <c r="J12" s="19">
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146"/>
-      <c r="B13" s="174"/>
-      <c r="C13" s="175">
+      <c r="A13" s="136"/>
+      <c r="B13" s="151"/>
+      <c r="C13" s="152">
         <v>9.5051183730503801E-5</v>
       </c>
       <c r="D13" s="21">
@@ -2918,552 +2817,213 @@
         <v>4209.62</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H13" s="21">
         <v>1.4E-3</v>
       </c>
-      <c r="I13" s="192" t="s">
-        <v>150</v>
+      <c r="I13" s="158" t="s">
+        <v>144</v>
       </c>
       <c r="J13" s="23">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="146"/>
-      <c r="B14" s="169" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="170"/>
-      <c r="D14" s="180">
+      <c r="A14" s="136"/>
+      <c r="B14" s="159" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="147">
+        <v>2.1800000000000001E-4</v>
+      </c>
+      <c r="D14" s="153">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E14" s="171"/>
-      <c r="F14" s="171"/>
-      <c r="G14" s="171"/>
-      <c r="H14" s="171"/>
-      <c r="I14" s="171"/>
-      <c r="J14" s="172"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="146"/>
-      <c r="B15" s="173"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="147"/>
-      <c r="B16" s="174"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="157" t="s">
+      <c r="E14" s="148">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="148">
+        <v>798.55</v>
+      </c>
+      <c r="G14" s="148" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="148">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="I14" s="148" t="s">
+        <v>154</v>
+      </c>
+      <c r="J14" s="149">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="136"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="141">
+        <v>1.45E-4</v>
+      </c>
+      <c r="D15" s="154"/>
+      <c r="E15" s="10">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3995.9</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15" s="10">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" s="19">
+        <v>5.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="126" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="169" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="171">
-        <v>2.7788500000000002E-3</v>
-      </c>
-      <c r="D17" s="171">
+      <c r="B16" s="146" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="147">
+        <v>2.7788499999999998E-3</v>
+      </c>
+      <c r="D16" s="148">
         <v>0.02</v>
       </c>
-      <c r="E17" s="180">
+      <c r="E16" s="153">
         <v>1000</v>
       </c>
-      <c r="F17" s="171">
+      <c r="F16" s="148">
         <v>906</v>
       </c>
-      <c r="G17" s="171" t="s">
+      <c r="G16" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="171">
+      <c r="H16" s="148">
         <v>6.6E-3</v>
       </c>
-      <c r="I17" s="171" t="s">
+      <c r="I16" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="172">
+      <c r="J16" s="149">
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="157"/>
-      <c r="B18" s="173"/>
-      <c r="C18" s="10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="126"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="141">
         <v>1.4983999999999999E-4</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D17" s="10">
         <v>0.01</v>
       </c>
-      <c r="E18" s="100"/>
-      <c r="F18" s="10">
+      <c r="E17" s="97"/>
+      <c r="F17" s="10">
         <v>1302</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H17" s="10">
         <v>1E-3</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J17" s="19">
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157"/>
-      <c r="B19" s="174"/>
-      <c r="C19" s="21">
+    <row r="18" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="126"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152">
         <v>1.8448E-4</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D18" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E19" s="100"/>
-      <c r="F19" s="21">
+      <c r="E18" s="97"/>
+      <c r="F18" s="21">
         <v>8802</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H18" s="21">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J18" s="23">
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="157"/>
-      <c r="B20" s="169" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="178"/>
-      <c r="D20" s="180">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="126"/>
+      <c r="B19" s="159" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="153" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="153">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E20" s="100"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="178"/>
-      <c r="H20" s="178"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="179"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="157"/>
-      <c r="B21" s="173"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="160"/>
-      <c r="G21" s="160"/>
-      <c r="H21" s="160"/>
-      <c r="I21" s="160"/>
-      <c r="J21" s="161"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="174"/>
-      <c r="C22" s="162"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="162"/>
-      <c r="H22" s="162"/>
-      <c r="I22" s="162"/>
-      <c r="J22" s="163"/>
-    </row>
-    <row r="24" spans="1:12" ht="22" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="22" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="140"/>
-      <c r="G28" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" s="63"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38">
+      <c r="E19" s="148">
         <v>1000</v>
       </c>
-      <c r="D29" s="144"/>
-      <c r="E29" s="142">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F29" s="139"/>
-      <c r="G29" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58">
-        <v>72.3</v>
-      </c>
-      <c r="L29" s="59"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="56"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38">
+      <c r="F19" s="148">
+        <v>1302</v>
+      </c>
+      <c r="G19" s="161" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="163"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="127"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="21">
         <v>5000</v>
       </c>
-      <c r="D30" s="144"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58">
-        <v>157.69999999999999</v>
-      </c>
-      <c r="L30" s="59"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38">
-        <v>1000</v>
-      </c>
-      <c r="D31" s="144"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="150" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" s="151"/>
-      <c r="I31" s="150" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="151"/>
-      <c r="K31" s="58">
-        <v>169.5</v>
-      </c>
-      <c r="L31" s="59"/>
-    </row>
-    <row r="32" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="57"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40">
-        <v>5000</v>
-      </c>
-      <c r="D32" s="145"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="141"/>
-      <c r="G32" s="148" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32" s="149"/>
-      <c r="I32" s="148" t="s">
-        <v>99</v>
-      </c>
-      <c r="J32" s="149"/>
-      <c r="K32" s="60">
-        <v>175.7</v>
-      </c>
-      <c r="L32" s="61"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-    </row>
-    <row r="34" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="154" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="152" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="153"/>
-      <c r="D35" s="153"/>
-      <c r="E35" s="153"/>
-      <c r="F35" s="153"/>
-      <c r="G35" s="153"/>
-      <c r="H35" s="153"/>
-      <c r="I35" s="153"/>
-      <c r="J35" s="154"/>
-    </row>
-    <row r="36" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="189"/>
-      <c r="B36" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="166" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="166" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="166" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="167" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="166" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="166" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="168" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="186" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="194" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" s="195">
-        <v>1.2558968979802399E-4</v>
-      </c>
-      <c r="D37" s="180">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E37" s="196">
-        <v>5</v>
-      </c>
-      <c r="F37" s="196">
-        <v>31.23</v>
-      </c>
-      <c r="G37" s="196" t="s">
-        <v>138</v>
-      </c>
-      <c r="H37" s="196">
-        <v>1.41E-2</v>
-      </c>
-      <c r="I37" s="196" t="s">
-        <v>139</v>
-      </c>
-      <c r="J37" s="197">
-        <v>0.11799999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="187"/>
-      <c r="B38" s="193" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="155"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="187"/>
-      <c r="B39" s="184"/>
-      <c r="C39" s="159"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="188"/>
-      <c r="B40" s="198"/>
-      <c r="C40" s="199"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="27"/>
-    </row>
-    <row r="41" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="182" t="s">
-        <v>134</v>
-      </c>
-      <c r="B41" s="194" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" s="100"/>
-      <c r="E41" s="180">
-        <v>1000</v>
-      </c>
-      <c r="F41" s="196">
-        <v>1302</v>
-      </c>
-      <c r="G41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="H41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="I41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="J41" s="197" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="182"/>
-      <c r="B42" s="193" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="176"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="100"/>
-      <c r="F42" s="176"/>
-      <c r="G42" s="176"/>
-      <c r="H42" s="176"/>
-      <c r="I42" s="176"/>
-      <c r="J42" s="177"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="182"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="160"/>
-      <c r="D43" s="100"/>
-      <c r="E43" s="100"/>
-      <c r="F43" s="160"/>
-      <c r="G43" s="160"/>
-      <c r="H43" s="160"/>
-      <c r="I43" s="160"/>
-      <c r="J43" s="161"/>
-    </row>
-    <row r="44" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="183"/>
-      <c r="B44" s="185"/>
-      <c r="C44" s="162"/>
-      <c r="D44" s="181"/>
-      <c r="E44" s="181"/>
-      <c r="F44" s="162"/>
-      <c r="G44" s="162"/>
-      <c r="H44" s="162"/>
-      <c r="I44" s="162"/>
-      <c r="J44" s="163"/>
+      <c r="F20" s="21">
+        <v>6151</v>
+      </c>
+      <c r="G20" s="165"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="166"/>
+      <c r="J20" s="131"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="D37:D44"/>
-    <mergeCell ref="E41:E44"/>
+  <mergeCells count="13">
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="B9:J9"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A11:A16"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="G19:J20"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
@@ -3477,8 +3037,8 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A41" zoomScale="173" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3528,18 +3088,18 @@
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="66" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -3568,8 +3128,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
-      <c r="B11" s="70">
+      <c r="A11" s="66"/>
+      <c r="B11" s="67">
         <v>1000</v>
       </c>
       <c r="C11" s="9">
@@ -3595,8 +3155,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3620,8 +3180,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="70"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="9">
         <v>0.01</v>
       </c>
@@ -3645,8 +3205,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="69"/>
-      <c r="B14" s="70">
+      <c r="A14" s="66"/>
+      <c r="B14" s="67">
         <v>5000</v>
       </c>
       <c r="C14" s="9">
@@ -3672,8 +3232,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3697,8 +3257,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="20">
         <v>0.01</v>
       </c>
@@ -3722,7 +3282,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -3751,8 +3311,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
-      <c r="B18" s="70">
+      <c r="A18" s="69"/>
+      <c r="B18" s="67">
         <v>1000</v>
       </c>
       <c r="C18" s="9">
@@ -3778,8 +3338,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="70"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="9">
         <v>0.01</v>
       </c>
@@ -3803,8 +3363,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="72"/>
-      <c r="B20" s="70"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3828,8 +3388,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
-      <c r="B21" s="70">
+      <c r="A21" s="69"/>
+      <c r="B21" s="67">
         <v>5000</v>
       </c>
       <c r="C21" s="9">
@@ -3855,8 +3415,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="72"/>
-      <c r="B22" s="70"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="9">
         <v>0.01</v>
       </c>
@@ -3880,8 +3440,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="137"/>
-      <c r="B23" s="71"/>
+      <c r="A23" s="134"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="24">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3905,7 +3465,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="125" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -3934,14 +3494,14 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="129"/>
-      <c r="B25" s="70">
+      <c r="A25" s="126"/>
+      <c r="B25" s="67">
         <v>1000</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D25" s="58">
+      <c r="D25" s="55">
         <v>16783</v>
       </c>
       <c r="E25" s="11">
@@ -3961,10 +3521,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="129"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="58"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="11">
         <v>1505</v>
       </c>
@@ -3982,10 +3542,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="129"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="58"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="11">
         <v>1725</v>
       </c>
@@ -4003,10 +3563,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="129"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="58"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="11">
         <v>1667</v>
       </c>
@@ -4024,10 +3584,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="129"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="58"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="11">
         <v>815</v>
       </c>
@@ -4045,10 +3605,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="129"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="58"/>
+      <c r="A30" s="126"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="11">
         <v>2029</v>
       </c>
@@ -4066,27 +3626,27 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="129"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="131" t="s">
+      <c r="A31" s="126"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="I31" s="132"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="129"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="129"/>
-      <c r="B32" s="71">
+      <c r="A32" s="126"/>
+      <c r="B32" s="68">
         <v>5000</v>
       </c>
-      <c r="C32" s="64">
+      <c r="C32" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D32" s="58">
+      <c r="D32" s="55">
         <v>45503</v>
       </c>
       <c r="E32" s="11">
@@ -4106,10 +3666,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="129"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="58"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="130"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="11">
         <v>1346</v>
       </c>
@@ -4127,10 +3687,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="129"/>
-      <c r="B34" s="133"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="58"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="130"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="11">
         <v>549</v>
       </c>
@@ -4148,10 +3708,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="129"/>
-      <c r="B35" s="133"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="58"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="11">
         <v>1630</v>
       </c>
@@ -4169,10 +3729,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="129"/>
-      <c r="B36" s="133"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="58"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="130"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="11">
         <v>101</v>
       </c>
@@ -4190,10 +3750,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="129"/>
-      <c r="B37" s="133"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="58"/>
+      <c r="A37" s="126"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="11">
         <v>1819</v>
       </c>
@@ -4211,27 +3771,27 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="129"/>
-      <c r="B38" s="134"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="135" t="s">
+      <c r="A38" s="126"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="136"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="132"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="133"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="129"/>
+      <c r="A39" s="126"/>
       <c r="B39" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="86" t="s">
+      <c r="C39" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="115"/>
+      <c r="D39" s="112"/>
       <c r="E39" s="33" t="s">
         <v>63</v>
       </c>
@@ -4241,86 +3801,86 @@
       <c r="G39" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="121"/>
-      <c r="I39" s="122"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="119"/>
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="129"/>
+      <c r="A40" s="126"/>
       <c r="B40" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="91"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="88"/>
       <c r="G40" s="11">
         <v>0.79820000000000002</v>
       </c>
-      <c r="H40" s="123"/>
-      <c r="I40" s="124"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="121"/>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="129"/>
+      <c r="A41" s="126"/>
       <c r="B41" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="91"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="88"/>
       <c r="G41" s="11">
         <v>0.20180000000000001</v>
       </c>
-      <c r="H41" s="123"/>
-      <c r="I41" s="124"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="121"/>
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="129"/>
+      <c r="A42" s="126"/>
       <c r="B42" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="76" t="s">
+      <c r="C42" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="91"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="88"/>
       <c r="G42" s="11">
         <v>0.75170000000000003</v>
       </c>
-      <c r="H42" s="123"/>
-      <c r="I42" s="124"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="121"/>
     </row>
     <row r="43" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="129"/>
+      <c r="A43" s="126"/>
       <c r="B43" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="80" t="s">
+      <c r="C43" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="79"/>
       <c r="G43" s="22">
         <v>0.24829999999999999</v>
       </c>
-      <c r="H43" s="125"/>
-      <c r="I43" s="126"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="123"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="129"/>
+      <c r="A44" s="126"/>
       <c r="B44" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="115"/>
+      <c r="D44" s="112"/>
       <c r="E44" s="33" t="s">
         <v>63</v>
       </c>
@@ -4333,83 +3893,83 @@
       <c r="H44" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I44" s="127"/>
+      <c r="I44" s="124"/>
     </row>
     <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="129"/>
+      <c r="A45" s="126"/>
       <c r="B45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C45" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="77"/>
-      <c r="E45" s="77"/>
-      <c r="F45" s="91"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="88"/>
       <c r="G45" s="11">
         <v>0.80359999999999998</v>
       </c>
       <c r="H45" s="11">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="I45" s="74"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="129"/>
+      <c r="A46" s="126"/>
       <c r="B46" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="91"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="88"/>
       <c r="G46" s="11">
         <v>0.19639999999999999</v>
       </c>
       <c r="H46" s="11">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="I46" s="74"/>
+      <c r="I46" s="71"/>
     </row>
     <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="129"/>
+      <c r="A47" s="126"/>
       <c r="B47" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="91"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="88"/>
       <c r="G47" s="11">
         <v>0.66900000000000004</v>
       </c>
       <c r="H47" s="11">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="I47" s="74"/>
+      <c r="I47" s="71"/>
     </row>
     <row r="48" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="130"/>
+      <c r="A48" s="127"/>
       <c r="B48" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="80" t="s">
+      <c r="C48" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="82"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
       <c r="G48" s="22">
         <v>0.33100000000000002</v>
       </c>
       <c r="H48" s="22">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="I48" s="75"/>
+      <c r="I48" s="72"/>
     </row>
     <row r="50" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
@@ -4435,215 +3995,215 @@
       <c r="C54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="62" t="s">
+      <c r="D54" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62" t="s">
+      <c r="E54" s="59"/>
+      <c r="F54" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62" t="s">
+      <c r="G54" s="59"/>
+      <c r="H54" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="I54" s="63"/>
+      <c r="I54" s="60"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="37">
         <v>1000</v>
       </c>
-      <c r="C55" s="64">
+      <c r="C55" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58" t="s">
+      <c r="E55" s="55"/>
+      <c r="F55" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58">
+      <c r="G55" s="55"/>
+      <c r="H55" s="55">
         <v>38.1</v>
       </c>
-      <c r="I55" s="59"/>
+      <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="56"/>
-      <c r="B56" s="38">
+      <c r="A56" s="53"/>
+      <c r="B56" s="37">
         <v>5000</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="58" t="s">
+      <c r="C56" s="61"/>
+      <c r="D56" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58" t="s">
+      <c r="E56" s="55"/>
+      <c r="F56" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58">
+      <c r="G56" s="55"/>
+      <c r="H56" s="55">
         <v>68.3</v>
       </c>
-      <c r="I56" s="59"/>
+      <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="37">
         <v>1000</v>
       </c>
-      <c r="C57" s="64"/>
-      <c r="D57" s="58" t="s">
+      <c r="C57" s="61"/>
+      <c r="D57" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58" t="s">
+      <c r="E57" s="55"/>
+      <c r="F57" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58">
+      <c r="G57" s="55"/>
+      <c r="H57" s="55">
         <v>35.700000000000003</v>
       </c>
-      <c r="I57" s="59"/>
+      <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="56"/>
-      <c r="B58" s="38">
+      <c r="A58" s="53"/>
+      <c r="B58" s="37">
         <v>5000</v>
       </c>
-      <c r="C58" s="64"/>
-      <c r="D58" s="58" t="s">
+      <c r="C58" s="61"/>
+      <c r="D58" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58" t="s">
+      <c r="E58" s="55"/>
+      <c r="F58" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58">
+      <c r="G58" s="55"/>
+      <c r="H58" s="55">
         <v>75.3</v>
       </c>
-      <c r="I58" s="59"/>
+      <c r="I58" s="56"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="38">
+      <c r="B59" s="37">
         <v>1000</v>
       </c>
-      <c r="C59" s="64"/>
-      <c r="D59" s="58" t="s">
+      <c r="C59" s="61"/>
+      <c r="D59" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58" t="s">
+      <c r="E59" s="55"/>
+      <c r="F59" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58">
+      <c r="G59" s="55"/>
+      <c r="H59" s="55">
         <v>72.3</v>
       </c>
-      <c r="I59" s="59"/>
+      <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="56"/>
-      <c r="B60" s="38">
+      <c r="A60" s="53"/>
+      <c r="B60" s="37">
         <v>5000</v>
       </c>
-      <c r="C60" s="64"/>
-      <c r="D60" s="58" t="s">
+      <c r="C60" s="61"/>
+      <c r="D60" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58" t="s">
+      <c r="E60" s="55"/>
+      <c r="F60" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58">
+      <c r="G60" s="55"/>
+      <c r="H60" s="55">
         <v>157.69999999999999</v>
       </c>
-      <c r="I60" s="59"/>
+      <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="37">
         <v>1000</v>
       </c>
-      <c r="C61" s="64"/>
-      <c r="D61" s="58" t="s">
+      <c r="C61" s="61"/>
+      <c r="D61" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58" t="s">
+      <c r="E61" s="55"/>
+      <c r="F61" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58">
+      <c r="G61" s="55"/>
+      <c r="H61" s="55">
         <v>169.5</v>
       </c>
-      <c r="I61" s="59"/>
+      <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
-      <c r="B62" s="40">
+      <c r="A62" s="54"/>
+      <c r="B62" s="38">
         <v>5000</v>
       </c>
-      <c r="C62" s="65"/>
-      <c r="D62" s="60" t="s">
+      <c r="C62" s="62"/>
+      <c r="D62" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="E62" s="60"/>
-      <c r="F62" s="60" t="s">
+      <c r="E62" s="57"/>
+      <c r="F62" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60">
+      <c r="G62" s="57"/>
+      <c r="H62" s="57">
         <v>175.7</v>
       </c>
-      <c r="I62" s="61"/>
+      <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="41"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="42"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
     </row>
     <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="42"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="42"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="42"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
     </row>
     <row r="66" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
@@ -4652,19 +4212,19 @@
       <c r="B66" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="42"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
+      <c r="I66" s="40"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="92" t="s">
+      <c r="A67" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="95">
+      <c r="B67" s="92">
         <v>15000</v>
       </c>
       <c r="C67" s="6" t="s">
@@ -4690,12 +4250,12 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="93"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="97">
+      <c r="A68" s="90"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="94">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D68" s="99">
+      <c r="D68" s="96">
         <v>634</v>
       </c>
       <c r="E68" s="11">
@@ -4715,10 +4275,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="93"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="98"/>
-      <c r="D69" s="100"/>
+      <c r="A69" s="90"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="97"/>
       <c r="E69" s="11">
         <v>919</v>
       </c>
@@ -4736,10 +4296,10 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="93"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="98"/>
-      <c r="D70" s="100"/>
+      <c r="A70" s="90"/>
+      <c r="B70" s="93"/>
+      <c r="C70" s="95"/>
+      <c r="D70" s="97"/>
       <c r="E70" s="11">
         <v>817</v>
       </c>
@@ -4757,10 +4317,10 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="93"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="98"/>
-      <c r="D71" s="100"/>
+      <c r="A71" s="90"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="97"/>
       <c r="E71" s="11">
         <v>1667</v>
       </c>
@@ -4778,10 +4338,10 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="93"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="98"/>
-      <c r="D72" s="100"/>
+      <c r="A72" s="90"/>
+      <c r="B72" s="93"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="97"/>
       <c r="E72" s="11">
         <v>119</v>
       </c>
@@ -4799,10 +4359,10 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="93"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="98"/>
-      <c r="D73" s="101"/>
+      <c r="A73" s="90"/>
+      <c r="B73" s="93"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="98"/>
       <c r="E73" s="11">
         <v>1366</v>
       </c>
@@ -4820,29 +4380,29 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="93"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="117"/>
+      <c r="A74" s="90"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="114"/>
       <c r="D74" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E74" s="118" t="s">
+      <c r="E74" s="115" t="s">
         <v>113</v>
       </c>
-      <c r="F74" s="119"/>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119"/>
-      <c r="I74" s="120"/>
+      <c r="F74" s="116"/>
+      <c r="G74" s="116"/>
+      <c r="H74" s="116"/>
+      <c r="I74" s="117"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="93"/>
+      <c r="A75" s="90"/>
       <c r="B75" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C75" s="105" t="s">
+      <c r="C75" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="D75" s="106"/>
+      <c r="D75" s="103"/>
       <c r="E75" s="33" t="s">
         <v>63</v>
       </c>
@@ -4852,87 +4412,87 @@
       <c r="G75" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="121"/>
-      <c r="I75" s="122"/>
+      <c r="H75" s="118"/>
+      <c r="I75" s="119"/>
     </row>
     <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="93"/>
+      <c r="A76" s="90"/>
       <c r="B76" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="C76" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D76" s="77"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="91"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="88"/>
       <c r="G76" s="11">
         <v>0.85440000000000005</v>
       </c>
-      <c r="H76" s="123"/>
-      <c r="I76" s="124"/>
+      <c r="H76" s="120"/>
+      <c r="I76" s="121"/>
     </row>
     <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="93"/>
+      <c r="A77" s="90"/>
       <c r="B77" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="C77" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D77" s="77"/>
-      <c r="E77" s="77"/>
-      <c r="F77" s="91"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="88"/>
       <c r="G77" s="11">
         <v>0.14560000000000001</v>
       </c>
-      <c r="H77" s="123"/>
-      <c r="I77" s="124"/>
+      <c r="H77" s="120"/>
+      <c r="I77" s="121"/>
     </row>
     <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="93"/>
+      <c r="A78" s="90"/>
       <c r="B78" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="76" t="s">
+      <c r="C78" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D78" s="77"/>
-      <c r="E78" s="77"/>
-      <c r="F78" s="91"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+      <c r="F78" s="88"/>
       <c r="G78" s="11">
         <v>1</v>
       </c>
-      <c r="H78" s="123"/>
-      <c r="I78" s="124"/>
+      <c r="H78" s="120"/>
+      <c r="I78" s="121"/>
     </row>
     <row r="79" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="93"/>
+      <c r="A79" s="90"/>
       <c r="B79" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="80" t="s">
+      <c r="C79" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="81"/>
-      <c r="E79" s="81"/>
-      <c r="F79" s="82"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="78"/>
+      <c r="F79" s="79"/>
       <c r="G79" s="22">
         <v>0</v>
       </c>
-      <c r="H79" s="125"/>
-      <c r="I79" s="126"/>
+      <c r="H79" s="122"/>
+      <c r="I79" s="123"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="93"/>
+      <c r="A80" s="90"/>
       <c r="B80" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C80" s="86" t="s">
+      <c r="C80" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="D80" s="115"/>
-      <c r="E80" s="45" t="s">
+      <c r="D80" s="112"/>
+      <c r="E80" s="42" t="s">
         <v>63</v>
       </c>
       <c r="F80" s="11">
@@ -4944,89 +4504,89 @@
       <c r="H80" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="I80" s="116"/>
+      <c r="I80" s="113"/>
     </row>
     <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="93"/>
+      <c r="A81" s="90"/>
       <c r="B81" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="76" t="s">
+      <c r="C81" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="91"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="88"/>
       <c r="G81" s="11">
         <v>0.83540000000000003</v>
       </c>
       <c r="H81" s="11">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I81" s="74"/>
+      <c r="I81" s="71"/>
     </row>
     <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="93"/>
+      <c r="A82" s="90"/>
       <c r="B82" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="76" t="s">
+      <c r="C82" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D82" s="77"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="91"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="88"/>
       <c r="G82" s="11">
         <v>0.1646</v>
       </c>
       <c r="H82" s="11">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I82" s="74"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="93"/>
+      <c r="A83" s="90"/>
       <c r="B83" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C83" s="76" t="s">
+      <c r="C83" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D83" s="77"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="91"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="88"/>
       <c r="G83" s="11">
         <v>0.84799999999999998</v>
       </c>
       <c r="H83" s="11">
         <v>0.1105</v>
       </c>
-      <c r="I83" s="74"/>
+      <c r="I83" s="71"/>
     </row>
     <row r="84" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="94"/>
+      <c r="A84" s="91"/>
       <c r="B84" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C84" s="80" t="s">
+      <c r="C84" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D84" s="81"/>
-      <c r="E84" s="81"/>
-      <c r="F84" s="82"/>
+      <c r="D84" s="78"/>
+      <c r="E84" s="78"/>
+      <c r="F84" s="79"/>
       <c r="G84" s="22">
         <v>0.152</v>
       </c>
       <c r="H84" s="22">
         <v>0.1105</v>
       </c>
-      <c r="I84" s="75"/>
+      <c r="I84" s="72"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="92" t="s">
+      <c r="A85" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="95">
+      <c r="B85" s="92">
         <v>15000</v>
       </c>
       <c r="C85" s="6" t="s">
@@ -5052,12 +4612,12 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="93"/>
-      <c r="B86" s="96"/>
-      <c r="C86" s="97">
+      <c r="A86" s="90"/>
+      <c r="B86" s="93"/>
+      <c r="C86" s="94">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D86" s="99">
+      <c r="D86" s="96">
         <v>580</v>
       </c>
       <c r="E86" s="11">
@@ -5077,10 +4637,10 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="93"/>
-      <c r="B87" s="96"/>
-      <c r="C87" s="98"/>
-      <c r="D87" s="100"/>
+      <c r="A87" s="90"/>
+      <c r="B87" s="93"/>
+      <c r="C87" s="95"/>
+      <c r="D87" s="97"/>
       <c r="E87" s="11">
         <v>608</v>
       </c>
@@ -5098,10 +4658,10 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="93"/>
-      <c r="B88" s="96"/>
-      <c r="C88" s="98"/>
-      <c r="D88" s="100"/>
+      <c r="A88" s="90"/>
+      <c r="B88" s="93"/>
+      <c r="C88" s="95"/>
+      <c r="D88" s="97"/>
       <c r="E88" s="11">
         <v>815</v>
       </c>
@@ -5119,10 +4679,10 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="93"/>
-      <c r="B89" s="96"/>
-      <c r="C89" s="98"/>
-      <c r="D89" s="100"/>
+      <c r="A89" s="90"/>
+      <c r="B89" s="93"/>
+      <c r="C89" s="95"/>
+      <c r="D89" s="97"/>
       <c r="E89" s="11">
         <v>1723</v>
       </c>
@@ -5140,10 +4700,10 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="93"/>
-      <c r="B90" s="96"/>
-      <c r="C90" s="98"/>
-      <c r="D90" s="100"/>
+      <c r="A90" s="90"/>
+      <c r="B90" s="93"/>
+      <c r="C90" s="95"/>
+      <c r="D90" s="97"/>
       <c r="E90" s="11">
         <v>101</v>
       </c>
@@ -5161,10 +4721,10 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="93"/>
-      <c r="B91" s="96"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="101"/>
+      <c r="A91" s="90"/>
+      <c r="B91" s="93"/>
+      <c r="C91" s="95"/>
+      <c r="D91" s="98"/>
       <c r="E91" s="11">
         <v>1494</v>
       </c>
@@ -5182,29 +4742,29 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="93"/>
-      <c r="B92" s="96"/>
-      <c r="C92" s="98"/>
+      <c r="A92" s="90"/>
+      <c r="B92" s="93"/>
+      <c r="C92" s="95"/>
       <c r="D92" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="E92" s="102" t="s">
+      <c r="E92" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="F92" s="103"/>
-      <c r="G92" s="103"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="104"/>
+      <c r="F92" s="100"/>
+      <c r="G92" s="100"/>
+      <c r="H92" s="100"/>
+      <c r="I92" s="101"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="93"/>
+      <c r="A93" s="90"/>
       <c r="B93" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C93" s="105" t="s">
+      <c r="C93" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="D93" s="106"/>
+      <c r="D93" s="103"/>
       <c r="E93" s="33" t="s">
         <v>63</v>
       </c>
@@ -5214,103 +4774,103 @@
       <c r="G93" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H93" s="107"/>
-      <c r="I93" s="108"/>
+      <c r="H93" s="104"/>
+      <c r="I93" s="105"/>
     </row>
     <row r="94" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="93"/>
-      <c r="B94" s="43" t="s">
+      <c r="A94" s="90"/>
+      <c r="B94" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="76" t="s">
+      <c r="C94" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D94" s="77"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="79"/>
-      <c r="G94" s="46">
+      <c r="D94" s="74"/>
+      <c r="E94" s="75"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="43">
         <v>0.75239999999999996</v>
       </c>
-      <c r="H94" s="109"/>
-      <c r="I94" s="110"/>
+      <c r="H94" s="106"/>
+      <c r="I94" s="107"/>
     </row>
     <row r="95" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="93"/>
-      <c r="B95" s="47" t="s">
+      <c r="A95" s="90"/>
+      <c r="B95" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C95" s="80" t="s">
+      <c r="C95" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D95" s="81"/>
-      <c r="E95" s="81"/>
-      <c r="F95" s="82"/>
-      <c r="G95" s="48">
+      <c r="D95" s="78"/>
+      <c r="E95" s="78"/>
+      <c r="F95" s="79"/>
+      <c r="G95" s="45">
         <v>0.24759999999999999</v>
       </c>
-      <c r="H95" s="111"/>
-      <c r="I95" s="112"/>
+      <c r="H95" s="108"/>
+      <c r="I95" s="109"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="93"/>
-      <c r="B96" s="49" t="s">
+      <c r="A96" s="90"/>
+      <c r="B96" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C96" s="113" t="s">
+      <c r="C96" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D96" s="114"/>
-      <c r="E96" s="50" t="s">
+      <c r="D96" s="111"/>
+      <c r="E96" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F96" s="51">
+      <c r="F96" s="48">
         <v>0.28689999999999999</v>
       </c>
-      <c r="G96" s="51" t="s">
+      <c r="G96" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="H96" s="52" t="s">
+      <c r="H96" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="I96" s="74"/>
+      <c r="I96" s="71"/>
     </row>
     <row r="97" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="93"/>
+      <c r="A97" s="90"/>
       <c r="B97" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C97" s="76" t="s">
+      <c r="C97" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D97" s="77"/>
-      <c r="E97" s="78"/>
-      <c r="F97" s="79"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="76"/>
       <c r="G97" s="11">
         <v>0.83509999999999995</v>
       </c>
       <c r="H97" s="11">
         <v>0.1114</v>
       </c>
-      <c r="I97" s="74"/>
+      <c r="I97" s="71"/>
     </row>
     <row r="98" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="94"/>
+      <c r="A98" s="91"/>
       <c r="B98" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C98" s="80" t="s">
+      <c r="C98" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D98" s="81"/>
-      <c r="E98" s="81"/>
-      <c r="F98" s="82"/>
+      <c r="D98" s="78"/>
+      <c r="E98" s="78"/>
+      <c r="F98" s="79"/>
       <c r="G98" s="22">
         <v>0.16489999999999999</v>
       </c>
       <c r="H98" s="22">
         <v>0.1114</v>
       </c>
-      <c r="I98" s="75"/>
+      <c r="I98" s="72"/>
     </row>
     <row r="100" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
@@ -5319,17 +4879,17 @@
     </row>
     <row r="101" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="83" t="s">
+      <c r="A102" s="80" t="s">
         <v>129</v>
       </c>
       <c r="B102" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C102" s="86" t="s">
+      <c r="C102" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D102" s="87"/>
-      <c r="E102" s="53" t="s">
+      <c r="D102" s="84"/>
+      <c r="E102" s="50" t="s">
         <v>131</v>
       </c>
       <c r="F102" s="34">
@@ -5338,86 +4898,86 @@
       <c r="G102" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="H102" s="54" t="s">
+      <c r="H102" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="I102" s="88"/>
+      <c r="I102" s="85"/>
     </row>
     <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="84"/>
-      <c r="B103" s="43" t="s">
+      <c r="A103" s="81"/>
+      <c r="B103" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C103" s="76" t="s">
+      <c r="C103" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D103" s="77"/>
-      <c r="E103" s="77"/>
-      <c r="F103" s="91"/>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
+      <c r="F103" s="88"/>
       <c r="G103" s="11">
         <v>0.83099999999999996</v>
       </c>
       <c r="H103" s="29">
         <v>3.04E-2</v>
       </c>
-      <c r="I103" s="89"/>
+      <c r="I103" s="86"/>
     </row>
     <row r="104" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="84"/>
-      <c r="B104" s="43" t="s">
+      <c r="A104" s="81"/>
+      <c r="B104" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C104" s="76" t="s">
+      <c r="C104" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D104" s="77"/>
-      <c r="E104" s="77"/>
-      <c r="F104" s="91"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="88"/>
       <c r="G104" s="11">
         <v>0.16900000000000001</v>
       </c>
       <c r="H104" s="29">
         <v>3.04E-2</v>
       </c>
-      <c r="I104" s="89"/>
+      <c r="I104" s="86"/>
     </row>
     <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="84"/>
-      <c r="B105" s="43" t="s">
+      <c r="A105" s="81"/>
+      <c r="B105" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C105" s="76" t="s">
+      <c r="C105" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D105" s="77"/>
-      <c r="E105" s="77"/>
-      <c r="F105" s="91"/>
+      <c r="D105" s="74"/>
+      <c r="E105" s="74"/>
+      <c r="F105" s="88"/>
       <c r="G105" s="11">
         <v>0.78990000000000005</v>
       </c>
       <c r="H105" s="29">
         <v>0.1716</v>
       </c>
-      <c r="I105" s="89"/>
+      <c r="I105" s="86"/>
     </row>
     <row r="106" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="85"/>
-      <c r="B106" s="47" t="s">
+      <c r="A106" s="82"/>
+      <c r="B106" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C106" s="80" t="s">
+      <c r="C106" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D106" s="81"/>
-      <c r="E106" s="81"/>
-      <c r="F106" s="82"/>
+      <c r="D106" s="78"/>
+      <c r="E106" s="78"/>
+      <c r="F106" s="79"/>
       <c r="G106" s="22">
         <v>0.21010000000000001</v>
       </c>
-      <c r="H106" s="55">
+      <c r="H106" s="52">
         <v>0.1716</v>
       </c>
-      <c r="I106" s="90"/>
+      <c r="I106" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="97">

</xml_diff>

<commit_message>
test optimization on Eduati2020 model
</commit_message>
<xml_diff>
--- a/Results/performance_vs_optPBN.xlsx
+++ b/Results/performance_vs_optPBN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luna/Desktop/Pancreatic cancer/BNMPy/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BE4CEF-9331-444E-98F8-F04E202AD69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5AE9A0-6221-4041-8DE4-7F4120BD898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1520" windowWidth="30220" windowHeight="20060" xr2:uid="{0F2A5497-3F2F-EF46-83BE-1532FE4FE77A}"/>
+    <workbookView xWindow="880" yWindow="840" windowWidth="33420" windowHeight="20060" xr2:uid="{0F2A5497-3F2F-EF46-83BE-1532FE4FE77A}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="157">
   <si>
     <t>*Note: Disc. = Discrete mode, Cont. = Continuous mode, Ext. = Extended model structure, Init. = Initial model tructure</t>
   </si>
@@ -809,24 +809,6 @@
     <t>0.6118, 0.3882</t>
   </si>
   <si>
-    <t>Model 3</t>
-  </si>
-  <si>
-    <t>Model 4</t>
-  </si>
-  <si>
-    <t>Particle swarm algorithm, PSO</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Differential evolution, DE</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>0.6991, 0.3009</t>
   </si>
   <si>
@@ -840,6 +822,42 @@
   </si>
   <si>
     <t>0.604, 0.3960</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>PSO</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>*Note:</t>
+  </si>
+  <si>
+    <t>iter. = iterations, Delta = difference between steady-state distributions and measurement data</t>
+  </si>
+  <si>
+    <t>Model: Trairatphisan2014</t>
+  </si>
+  <si>
+    <t>iter.</t>
+  </si>
+  <si>
+    <t>Not provided</t>
+  </si>
+  <si>
+    <t>0.7039, 0.2961</t>
+  </si>
+  <si>
+    <t>0.5901, 0.4099</t>
+  </si>
+  <si>
+    <t>0.7009, 0.2991</t>
+  </si>
+  <si>
+    <t>0.5948, 0.4052</t>
   </si>
 </sst>
 </file>
@@ -956,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="69">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -1720,27 +1738,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1781,36 +1782,17 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1820,7 +1802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1924,15 +1906,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1943,9 +1919,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2230,45 +2203,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2278,93 +2215,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2376,25 +2272,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2734,10 +2633,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2767,13 +2666,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -2785,7 +2684,7 @@
     </row>
     <row r="7" spans="1:11" ht="22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" t="s">
@@ -2793,91 +2692,91 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="154" t="s">
+    <row r="9" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="155" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="154"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="139"/>
     </row>
     <row r="10" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="189"/>
-      <c r="B10" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="166" t="s">
+      <c r="A10" s="164"/>
+      <c r="B10" s="142" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="143" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="166" t="s">
+      <c r="E10" s="143" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="167" t="s">
+      <c r="G10" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="166" t="s">
+      <c r="H10" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="166" t="s">
+      <c r="I10" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="168" t="s">
+      <c r="J10" s="145" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="156" t="s">
+      <c r="A11" s="140" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="169" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="170">
+      <c r="B11" s="146" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="147">
         <v>1.2558968979802399E-4</v>
       </c>
-      <c r="D11" s="171">
+      <c r="D11" s="148">
         <v>0.02</v>
       </c>
-      <c r="E11" s="171">
+      <c r="E11" s="148">
         <v>5</v>
       </c>
-      <c r="F11" s="171">
+      <c r="F11" s="148">
         <v>31.23</v>
       </c>
-      <c r="G11" s="171" t="s">
+      <c r="G11" s="148" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="171">
+      <c r="H11" s="148">
         <v>1.41E-2</v>
       </c>
-      <c r="I11" s="190" t="s">
+      <c r="I11" s="156" t="s">
         <v>139</v>
       </c>
-      <c r="J11" s="172">
-        <v>0.11799999999999999</v>
+      <c r="J11" s="149">
+        <v>1.18E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="146"/>
-      <c r="B12" s="173"/>
-      <c r="C12" s="159">
+      <c r="A12" s="136"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="141">
         <v>1.3409822281216599E-4</v>
       </c>
       <c r="D12" s="10">
@@ -2890,22 +2789,22 @@
         <v>1105.58</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H12" s="10">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I12" s="191" t="s">
-        <v>147</v>
+      <c r="I12" s="157" t="s">
+        <v>141</v>
       </c>
       <c r="J12" s="19">
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146"/>
-      <c r="B13" s="174"/>
-      <c r="C13" s="175">
+      <c r="A13" s="136"/>
+      <c r="B13" s="151"/>
+      <c r="C13" s="152">
         <v>9.5051183730503801E-5</v>
       </c>
       <c r="D13" s="21">
@@ -2918,552 +2817,213 @@
         <v>4209.62</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H13" s="21">
         <v>1.4E-3</v>
       </c>
-      <c r="I13" s="192" t="s">
-        <v>150</v>
+      <c r="I13" s="158" t="s">
+        <v>144</v>
       </c>
       <c r="J13" s="23">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="146"/>
-      <c r="B14" s="169" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="170"/>
-      <c r="D14" s="180">
+      <c r="A14" s="136"/>
+      <c r="B14" s="159" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="147">
+        <v>2.1800000000000001E-4</v>
+      </c>
+      <c r="D14" s="153">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E14" s="171"/>
-      <c r="F14" s="171"/>
-      <c r="G14" s="171"/>
-      <c r="H14" s="171"/>
-      <c r="I14" s="171"/>
-      <c r="J14" s="172"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="146"/>
-      <c r="B15" s="173"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="147"/>
-      <c r="B16" s="174"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="157" t="s">
+      <c r="E14" s="148">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="148">
+        <v>798.55</v>
+      </c>
+      <c r="G14" s="148" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="148">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="I14" s="148" t="s">
+        <v>154</v>
+      </c>
+      <c r="J14" s="149">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="136"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="141">
+        <v>1.45E-4</v>
+      </c>
+      <c r="D15" s="154"/>
+      <c r="E15" s="10">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3995.9</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15" s="10">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" s="19">
+        <v>5.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="126" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="169" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="171">
-        <v>2.7788500000000002E-3</v>
-      </c>
-      <c r="D17" s="171">
+      <c r="B16" s="146" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="147">
+        <v>2.7788499999999998E-3</v>
+      </c>
+      <c r="D16" s="148">
         <v>0.02</v>
       </c>
-      <c r="E17" s="180">
+      <c r="E16" s="153">
         <v>1000</v>
       </c>
-      <c r="F17" s="171">
+      <c r="F16" s="148">
         <v>906</v>
       </c>
-      <c r="G17" s="171" t="s">
+      <c r="G16" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="171">
+      <c r="H16" s="148">
         <v>6.6E-3</v>
       </c>
-      <c r="I17" s="171" t="s">
+      <c r="I16" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="172">
+      <c r="J16" s="149">
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="157"/>
-      <c r="B18" s="173"/>
-      <c r="C18" s="10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="126"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="141">
         <v>1.4983999999999999E-4</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D17" s="10">
         <v>0.01</v>
       </c>
-      <c r="E18" s="100"/>
-      <c r="F18" s="10">
+      <c r="E17" s="97"/>
+      <c r="F17" s="10">
         <v>1302</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H17" s="10">
         <v>1E-3</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J17" s="19">
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157"/>
-      <c r="B19" s="174"/>
-      <c r="C19" s="21">
+    <row r="18" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="126"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152">
         <v>1.8448E-4</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D18" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E19" s="100"/>
-      <c r="F19" s="21">
+      <c r="E18" s="97"/>
+      <c r="F18" s="21">
         <v>8802</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H18" s="21">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J18" s="23">
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="157"/>
-      <c r="B20" s="169" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="178"/>
-      <c r="D20" s="180">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="126"/>
+      <c r="B19" s="159" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="153" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="153">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E20" s="100"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="178"/>
-      <c r="H20" s="178"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="179"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="157"/>
-      <c r="B21" s="173"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="160"/>
-      <c r="G21" s="160"/>
-      <c r="H21" s="160"/>
-      <c r="I21" s="160"/>
-      <c r="J21" s="161"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="174"/>
-      <c r="C22" s="162"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="162"/>
-      <c r="H22" s="162"/>
-      <c r="I22" s="162"/>
-      <c r="J22" s="163"/>
-    </row>
-    <row r="24" spans="1:12" ht="22" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="22" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="140"/>
-      <c r="G28" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" s="63"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38">
+      <c r="E19" s="148">
         <v>1000</v>
       </c>
-      <c r="D29" s="144"/>
-      <c r="E29" s="142">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F29" s="139"/>
-      <c r="G29" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58">
-        <v>72.3</v>
-      </c>
-      <c r="L29" s="59"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="56"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38">
+      <c r="F19" s="148">
+        <v>1302</v>
+      </c>
+      <c r="G19" s="161" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="163"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="127"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="21">
         <v>5000</v>
       </c>
-      <c r="D30" s="144"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58">
-        <v>157.69999999999999</v>
-      </c>
-      <c r="L30" s="59"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38">
-        <v>1000</v>
-      </c>
-      <c r="D31" s="144"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="150" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" s="151"/>
-      <c r="I31" s="150" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="151"/>
-      <c r="K31" s="58">
-        <v>169.5</v>
-      </c>
-      <c r="L31" s="59"/>
-    </row>
-    <row r="32" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="57"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40">
-        <v>5000</v>
-      </c>
-      <c r="D32" s="145"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="141"/>
-      <c r="G32" s="148" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32" s="149"/>
-      <c r="I32" s="148" t="s">
-        <v>99</v>
-      </c>
-      <c r="J32" s="149"/>
-      <c r="K32" s="60">
-        <v>175.7</v>
-      </c>
-      <c r="L32" s="61"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-    </row>
-    <row r="34" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="154" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="152" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="153"/>
-      <c r="D35" s="153"/>
-      <c r="E35" s="153"/>
-      <c r="F35" s="153"/>
-      <c r="G35" s="153"/>
-      <c r="H35" s="153"/>
-      <c r="I35" s="153"/>
-      <c r="J35" s="154"/>
-    </row>
-    <row r="36" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="189"/>
-      <c r="B36" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="166" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="166" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="166" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="167" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="166" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="166" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="168" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="186" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="194" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" s="195">
-        <v>1.2558968979802399E-4</v>
-      </c>
-      <c r="D37" s="180">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E37" s="196">
-        <v>5</v>
-      </c>
-      <c r="F37" s="196">
-        <v>31.23</v>
-      </c>
-      <c r="G37" s="196" t="s">
-        <v>138</v>
-      </c>
-      <c r="H37" s="196">
-        <v>1.41E-2</v>
-      </c>
-      <c r="I37" s="196" t="s">
-        <v>139</v>
-      </c>
-      <c r="J37" s="197">
-        <v>0.11799999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="187"/>
-      <c r="B38" s="193" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="155"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="187"/>
-      <c r="B39" s="184"/>
-      <c r="C39" s="159"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="188"/>
-      <c r="B40" s="198"/>
-      <c r="C40" s="199"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="27"/>
-    </row>
-    <row r="41" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="182" t="s">
-        <v>134</v>
-      </c>
-      <c r="B41" s="194" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" s="100"/>
-      <c r="E41" s="180">
-        <v>1000</v>
-      </c>
-      <c r="F41" s="196">
-        <v>1302</v>
-      </c>
-      <c r="G41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="H41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="I41" s="196" t="s">
-        <v>145</v>
-      </c>
-      <c r="J41" s="197" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="182"/>
-      <c r="B42" s="193" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="176"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="100"/>
-      <c r="F42" s="176"/>
-      <c r="G42" s="176"/>
-      <c r="H42" s="176"/>
-      <c r="I42" s="176"/>
-      <c r="J42" s="177"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="182"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="160"/>
-      <c r="D43" s="100"/>
-      <c r="E43" s="100"/>
-      <c r="F43" s="160"/>
-      <c r="G43" s="160"/>
-      <c r="H43" s="160"/>
-      <c r="I43" s="160"/>
-      <c r="J43" s="161"/>
-    </row>
-    <row r="44" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="183"/>
-      <c r="B44" s="185"/>
-      <c r="C44" s="162"/>
-      <c r="D44" s="181"/>
-      <c r="E44" s="181"/>
-      <c r="F44" s="162"/>
-      <c r="G44" s="162"/>
-      <c r="H44" s="162"/>
-      <c r="I44" s="162"/>
-      <c r="J44" s="163"/>
+      <c r="F20" s="21">
+        <v>6151</v>
+      </c>
+      <c r="G20" s="165"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="166"/>
+      <c r="J20" s="131"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="D37:D44"/>
-    <mergeCell ref="E41:E44"/>
+  <mergeCells count="13">
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="B9:J9"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A11:A16"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="G19:J20"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
@@ -3477,8 +3037,8 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A41" zoomScale="173" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3528,18 +3088,18 @@
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="66" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -3568,8 +3128,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
-      <c r="B11" s="70">
+      <c r="A11" s="66"/>
+      <c r="B11" s="67">
         <v>1000</v>
       </c>
       <c r="C11" s="9">
@@ -3595,8 +3155,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3620,8 +3180,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="70"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="9">
         <v>0.01</v>
       </c>
@@ -3645,8 +3205,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="69"/>
-      <c r="B14" s="70">
+      <c r="A14" s="66"/>
+      <c r="B14" s="67">
         <v>5000</v>
       </c>
       <c r="C14" s="9">
@@ -3672,8 +3232,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3697,8 +3257,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="20">
         <v>0.01</v>
       </c>
@@ -3722,7 +3282,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -3751,8 +3311,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
-      <c r="B18" s="70">
+      <c r="A18" s="69"/>
+      <c r="B18" s="67">
         <v>1000</v>
       </c>
       <c r="C18" s="9">
@@ -3778,8 +3338,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="70"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="9">
         <v>0.01</v>
       </c>
@@ -3803,8 +3363,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="72"/>
-      <c r="B20" s="70"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3828,8 +3388,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
-      <c r="B21" s="70">
+      <c r="A21" s="69"/>
+      <c r="B21" s="67">
         <v>5000</v>
       </c>
       <c r="C21" s="9">
@@ -3855,8 +3415,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="72"/>
-      <c r="B22" s="70"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="9">
         <v>0.01</v>
       </c>
@@ -3880,8 +3440,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="137"/>
-      <c r="B23" s="71"/>
+      <c r="A23" s="134"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="24">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3905,7 +3465,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="125" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -3934,14 +3494,14 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="129"/>
-      <c r="B25" s="70">
+      <c r="A25" s="126"/>
+      <c r="B25" s="67">
         <v>1000</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D25" s="58">
+      <c r="D25" s="55">
         <v>16783</v>
       </c>
       <c r="E25" s="11">
@@ -3961,10 +3521,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="129"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="58"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="11">
         <v>1505</v>
       </c>
@@ -3982,10 +3542,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="129"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="58"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="11">
         <v>1725</v>
       </c>
@@ -4003,10 +3563,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="129"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="58"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="11">
         <v>1667</v>
       </c>
@@ -4024,10 +3584,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="129"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="58"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="11">
         <v>815</v>
       </c>
@@ -4045,10 +3605,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="129"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="58"/>
+      <c r="A30" s="126"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="11">
         <v>2029</v>
       </c>
@@ -4066,27 +3626,27 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="129"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="131" t="s">
+      <c r="A31" s="126"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="I31" s="132"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="129"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="129"/>
-      <c r="B32" s="71">
+      <c r="A32" s="126"/>
+      <c r="B32" s="68">
         <v>5000</v>
       </c>
-      <c r="C32" s="64">
+      <c r="C32" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D32" s="58">
+      <c r="D32" s="55">
         <v>45503</v>
       </c>
       <c r="E32" s="11">
@@ -4106,10 +3666,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="129"/>
-      <c r="B33" s="133"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="58"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="130"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="11">
         <v>1346</v>
       </c>
@@ -4127,10 +3687,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="129"/>
-      <c r="B34" s="133"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="58"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="130"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="11">
         <v>549</v>
       </c>
@@ -4148,10 +3708,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="129"/>
-      <c r="B35" s="133"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="58"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="11">
         <v>1630</v>
       </c>
@@ -4169,10 +3729,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="129"/>
-      <c r="B36" s="133"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="58"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="130"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="11">
         <v>101</v>
       </c>
@@ -4190,10 +3750,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="129"/>
-      <c r="B37" s="133"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="58"/>
+      <c r="A37" s="126"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="11">
         <v>1819</v>
       </c>
@@ -4211,27 +3771,27 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="129"/>
-      <c r="B38" s="134"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="135" t="s">
+      <c r="A38" s="126"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="136"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="132"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="133"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="129"/>
+      <c r="A39" s="126"/>
       <c r="B39" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="86" t="s">
+      <c r="C39" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="115"/>
+      <c r="D39" s="112"/>
       <c r="E39" s="33" t="s">
         <v>63</v>
       </c>
@@ -4241,86 +3801,86 @@
       <c r="G39" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="121"/>
-      <c r="I39" s="122"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="119"/>
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="129"/>
+      <c r="A40" s="126"/>
       <c r="B40" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="91"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="88"/>
       <c r="G40" s="11">
         <v>0.79820000000000002</v>
       </c>
-      <c r="H40" s="123"/>
-      <c r="I40" s="124"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="121"/>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="129"/>
+      <c r="A41" s="126"/>
       <c r="B41" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="91"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="88"/>
       <c r="G41" s="11">
         <v>0.20180000000000001</v>
       </c>
-      <c r="H41" s="123"/>
-      <c r="I41" s="124"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="121"/>
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="129"/>
+      <c r="A42" s="126"/>
       <c r="B42" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="76" t="s">
+      <c r="C42" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="91"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="88"/>
       <c r="G42" s="11">
         <v>0.75170000000000003</v>
       </c>
-      <c r="H42" s="123"/>
-      <c r="I42" s="124"/>
+      <c r="H42" s="120"/>
+      <c r="I42" s="121"/>
     </row>
     <row r="43" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="129"/>
+      <c r="A43" s="126"/>
       <c r="B43" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="80" t="s">
+      <c r="C43" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="79"/>
       <c r="G43" s="22">
         <v>0.24829999999999999</v>
       </c>
-      <c r="H43" s="125"/>
-      <c r="I43" s="126"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="123"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="129"/>
+      <c r="A44" s="126"/>
       <c r="B44" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="115"/>
+      <c r="D44" s="112"/>
       <c r="E44" s="33" t="s">
         <v>63</v>
       </c>
@@ -4333,83 +3893,83 @@
       <c r="H44" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I44" s="127"/>
+      <c r="I44" s="124"/>
     </row>
     <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="129"/>
+      <c r="A45" s="126"/>
       <c r="B45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C45" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="77"/>
-      <c r="E45" s="77"/>
-      <c r="F45" s="91"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="88"/>
       <c r="G45" s="11">
         <v>0.80359999999999998</v>
       </c>
       <c r="H45" s="11">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="I45" s="74"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="129"/>
+      <c r="A46" s="126"/>
       <c r="B46" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="91"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="88"/>
       <c r="G46" s="11">
         <v>0.19639999999999999</v>
       </c>
       <c r="H46" s="11">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="I46" s="74"/>
+      <c r="I46" s="71"/>
     </row>
     <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="129"/>
+      <c r="A47" s="126"/>
       <c r="B47" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="91"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="88"/>
       <c r="G47" s="11">
         <v>0.66900000000000004</v>
       </c>
       <c r="H47" s="11">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="I47" s="74"/>
+      <c r="I47" s="71"/>
     </row>
     <row r="48" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="130"/>
+      <c r="A48" s="127"/>
       <c r="B48" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="80" t="s">
+      <c r="C48" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="82"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
       <c r="G48" s="22">
         <v>0.33100000000000002</v>
       </c>
       <c r="H48" s="22">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="I48" s="75"/>
+      <c r="I48" s="72"/>
     </row>
     <row r="50" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
@@ -4435,215 +3995,215 @@
       <c r="C54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="62" t="s">
+      <c r="D54" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62" t="s">
+      <c r="E54" s="59"/>
+      <c r="F54" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62" t="s">
+      <c r="G54" s="59"/>
+      <c r="H54" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="I54" s="63"/>
+      <c r="I54" s="60"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="37">
         <v>1000</v>
       </c>
-      <c r="C55" s="64">
+      <c r="C55" s="61">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58" t="s">
+      <c r="E55" s="55"/>
+      <c r="F55" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58">
+      <c r="G55" s="55"/>
+      <c r="H55" s="55">
         <v>38.1</v>
       </c>
-      <c r="I55" s="59"/>
+      <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="56"/>
-      <c r="B56" s="38">
+      <c r="A56" s="53"/>
+      <c r="B56" s="37">
         <v>5000</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="58" t="s">
+      <c r="C56" s="61"/>
+      <c r="D56" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58" t="s">
+      <c r="E56" s="55"/>
+      <c r="F56" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58">
+      <c r="G56" s="55"/>
+      <c r="H56" s="55">
         <v>68.3</v>
       </c>
-      <c r="I56" s="59"/>
+      <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="37">
         <v>1000</v>
       </c>
-      <c r="C57" s="64"/>
-      <c r="D57" s="58" t="s">
+      <c r="C57" s="61"/>
+      <c r="D57" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58" t="s">
+      <c r="E57" s="55"/>
+      <c r="F57" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58">
+      <c r="G57" s="55"/>
+      <c r="H57" s="55">
         <v>35.700000000000003</v>
       </c>
-      <c r="I57" s="59"/>
+      <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="56"/>
-      <c r="B58" s="38">
+      <c r="A58" s="53"/>
+      <c r="B58" s="37">
         <v>5000</v>
       </c>
-      <c r="C58" s="64"/>
-      <c r="D58" s="58" t="s">
+      <c r="C58" s="61"/>
+      <c r="D58" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58" t="s">
+      <c r="E58" s="55"/>
+      <c r="F58" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58">
+      <c r="G58" s="55"/>
+      <c r="H58" s="55">
         <v>75.3</v>
       </c>
-      <c r="I58" s="59"/>
+      <c r="I58" s="56"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="38">
+      <c r="B59" s="37">
         <v>1000</v>
       </c>
-      <c r="C59" s="64"/>
-      <c r="D59" s="58" t="s">
+      <c r="C59" s="61"/>
+      <c r="D59" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58" t="s">
+      <c r="E59" s="55"/>
+      <c r="F59" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58">
+      <c r="G59" s="55"/>
+      <c r="H59" s="55">
         <v>72.3</v>
       </c>
-      <c r="I59" s="59"/>
+      <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="56"/>
-      <c r="B60" s="38">
+      <c r="A60" s="53"/>
+      <c r="B60" s="37">
         <v>5000</v>
       </c>
-      <c r="C60" s="64"/>
-      <c r="D60" s="58" t="s">
+      <c r="C60" s="61"/>
+      <c r="D60" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58" t="s">
+      <c r="E60" s="55"/>
+      <c r="F60" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58">
+      <c r="G60" s="55"/>
+      <c r="H60" s="55">
         <v>157.69999999999999</v>
       </c>
-      <c r="I60" s="59"/>
+      <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="37">
         <v>1000</v>
       </c>
-      <c r="C61" s="64"/>
-      <c r="D61" s="58" t="s">
+      <c r="C61" s="61"/>
+      <c r="D61" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58" t="s">
+      <c r="E61" s="55"/>
+      <c r="F61" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58">
+      <c r="G61" s="55"/>
+      <c r="H61" s="55">
         <v>169.5</v>
       </c>
-      <c r="I61" s="59"/>
+      <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
-      <c r="B62" s="40">
+      <c r="A62" s="54"/>
+      <c r="B62" s="38">
         <v>5000</v>
       </c>
-      <c r="C62" s="65"/>
-      <c r="D62" s="60" t="s">
+      <c r="C62" s="62"/>
+      <c r="D62" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="E62" s="60"/>
-      <c r="F62" s="60" t="s">
+      <c r="E62" s="57"/>
+      <c r="F62" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60">
+      <c r="G62" s="57"/>
+      <c r="H62" s="57">
         <v>175.7</v>
       </c>
-      <c r="I62" s="61"/>
+      <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="41"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="42"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
     </row>
     <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="42"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="42"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
     </row>
     <row r="65" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="42"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
     </row>
     <row r="66" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
@@ -4652,19 +4212,19 @@
       <c r="B66" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="42"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
+      <c r="I66" s="40"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="92" t="s">
+      <c r="A67" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="95">
+      <c r="B67" s="92">
         <v>15000</v>
       </c>
       <c r="C67" s="6" t="s">
@@ -4690,12 +4250,12 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="93"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="97">
+      <c r="A68" s="90"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="94">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D68" s="99">
+      <c r="D68" s="96">
         <v>634</v>
       </c>
       <c r="E68" s="11">
@@ -4715,10 +4275,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="93"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="98"/>
-      <c r="D69" s="100"/>
+      <c r="A69" s="90"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="97"/>
       <c r="E69" s="11">
         <v>919</v>
       </c>
@@ -4736,10 +4296,10 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="93"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="98"/>
-      <c r="D70" s="100"/>
+      <c r="A70" s="90"/>
+      <c r="B70" s="93"/>
+      <c r="C70" s="95"/>
+      <c r="D70" s="97"/>
       <c r="E70" s="11">
         <v>817</v>
       </c>
@@ -4757,10 +4317,10 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="93"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="98"/>
-      <c r="D71" s="100"/>
+      <c r="A71" s="90"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="97"/>
       <c r="E71" s="11">
         <v>1667</v>
       </c>
@@ -4778,10 +4338,10 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="93"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="98"/>
-      <c r="D72" s="100"/>
+      <c r="A72" s="90"/>
+      <c r="B72" s="93"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="97"/>
       <c r="E72" s="11">
         <v>119</v>
       </c>
@@ -4799,10 +4359,10 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="93"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="98"/>
-      <c r="D73" s="101"/>
+      <c r="A73" s="90"/>
+      <c r="B73" s="93"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="98"/>
       <c r="E73" s="11">
         <v>1366</v>
       </c>
@@ -4820,29 +4380,29 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="93"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="117"/>
+      <c r="A74" s="90"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="114"/>
       <c r="D74" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E74" s="118" t="s">
+      <c r="E74" s="115" t="s">
         <v>113</v>
       </c>
-      <c r="F74" s="119"/>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119"/>
-      <c r="I74" s="120"/>
+      <c r="F74" s="116"/>
+      <c r="G74" s="116"/>
+      <c r="H74" s="116"/>
+      <c r="I74" s="117"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="93"/>
+      <c r="A75" s="90"/>
       <c r="B75" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C75" s="105" t="s">
+      <c r="C75" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="D75" s="106"/>
+      <c r="D75" s="103"/>
       <c r="E75" s="33" t="s">
         <v>63</v>
       </c>
@@ -4852,87 +4412,87 @@
       <c r="G75" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="121"/>
-      <c r="I75" s="122"/>
+      <c r="H75" s="118"/>
+      <c r="I75" s="119"/>
     </row>
     <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="93"/>
+      <c r="A76" s="90"/>
       <c r="B76" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="C76" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D76" s="77"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="91"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="88"/>
       <c r="G76" s="11">
         <v>0.85440000000000005</v>
       </c>
-      <c r="H76" s="123"/>
-      <c r="I76" s="124"/>
+      <c r="H76" s="120"/>
+      <c r="I76" s="121"/>
     </row>
     <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="93"/>
+      <c r="A77" s="90"/>
       <c r="B77" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="C77" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D77" s="77"/>
-      <c r="E77" s="77"/>
-      <c r="F77" s="91"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="88"/>
       <c r="G77" s="11">
         <v>0.14560000000000001</v>
       </c>
-      <c r="H77" s="123"/>
-      <c r="I77" s="124"/>
+      <c r="H77" s="120"/>
+      <c r="I77" s="121"/>
     </row>
     <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="93"/>
+      <c r="A78" s="90"/>
       <c r="B78" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="76" t="s">
+      <c r="C78" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D78" s="77"/>
-      <c r="E78" s="77"/>
-      <c r="F78" s="91"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+      <c r="F78" s="88"/>
       <c r="G78" s="11">
         <v>1</v>
       </c>
-      <c r="H78" s="123"/>
-      <c r="I78" s="124"/>
+      <c r="H78" s="120"/>
+      <c r="I78" s="121"/>
     </row>
     <row r="79" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="93"/>
+      <c r="A79" s="90"/>
       <c r="B79" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="80" t="s">
+      <c r="C79" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="81"/>
-      <c r="E79" s="81"/>
-      <c r="F79" s="82"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="78"/>
+      <c r="F79" s="79"/>
       <c r="G79" s="22">
         <v>0</v>
       </c>
-      <c r="H79" s="125"/>
-      <c r="I79" s="126"/>
+      <c r="H79" s="122"/>
+      <c r="I79" s="123"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="93"/>
+      <c r="A80" s="90"/>
       <c r="B80" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C80" s="86" t="s">
+      <c r="C80" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="D80" s="115"/>
-      <c r="E80" s="45" t="s">
+      <c r="D80" s="112"/>
+      <c r="E80" s="42" t="s">
         <v>63</v>
       </c>
       <c r="F80" s="11">
@@ -4944,89 +4504,89 @@
       <c r="H80" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="I80" s="116"/>
+      <c r="I80" s="113"/>
     </row>
     <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="93"/>
+      <c r="A81" s="90"/>
       <c r="B81" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="76" t="s">
+      <c r="C81" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="91"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="88"/>
       <c r="G81" s="11">
         <v>0.83540000000000003</v>
       </c>
       <c r="H81" s="11">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I81" s="74"/>
+      <c r="I81" s="71"/>
     </row>
     <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="93"/>
+      <c r="A82" s="90"/>
       <c r="B82" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="76" t="s">
+      <c r="C82" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D82" s="77"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="91"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="88"/>
       <c r="G82" s="11">
         <v>0.1646</v>
       </c>
       <c r="H82" s="11">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="I82" s="74"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="93"/>
+      <c r="A83" s="90"/>
       <c r="B83" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C83" s="76" t="s">
+      <c r="C83" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D83" s="77"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="91"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="88"/>
       <c r="G83" s="11">
         <v>0.84799999999999998</v>
       </c>
       <c r="H83" s="11">
         <v>0.1105</v>
       </c>
-      <c r="I83" s="74"/>
+      <c r="I83" s="71"/>
     </row>
     <row r="84" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="94"/>
+      <c r="A84" s="91"/>
       <c r="B84" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C84" s="80" t="s">
+      <c r="C84" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D84" s="81"/>
-      <c r="E84" s="81"/>
-      <c r="F84" s="82"/>
+      <c r="D84" s="78"/>
+      <c r="E84" s="78"/>
+      <c r="F84" s="79"/>
       <c r="G84" s="22">
         <v>0.152</v>
       </c>
       <c r="H84" s="22">
         <v>0.1105</v>
       </c>
-      <c r="I84" s="75"/>
+      <c r="I84" s="72"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="92" t="s">
+      <c r="A85" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="95">
+      <c r="B85" s="92">
         <v>15000</v>
       </c>
       <c r="C85" s="6" t="s">
@@ -5052,12 +4612,12 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="93"/>
-      <c r="B86" s="96"/>
-      <c r="C86" s="97">
+      <c r="A86" s="90"/>
+      <c r="B86" s="93"/>
+      <c r="C86" s="94">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D86" s="99">
+      <c r="D86" s="96">
         <v>580</v>
       </c>
       <c r="E86" s="11">
@@ -5077,10 +4637,10 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="93"/>
-      <c r="B87" s="96"/>
-      <c r="C87" s="98"/>
-      <c r="D87" s="100"/>
+      <c r="A87" s="90"/>
+      <c r="B87" s="93"/>
+      <c r="C87" s="95"/>
+      <c r="D87" s="97"/>
       <c r="E87" s="11">
         <v>608</v>
       </c>
@@ -5098,10 +4658,10 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="93"/>
-      <c r="B88" s="96"/>
-      <c r="C88" s="98"/>
-      <c r="D88" s="100"/>
+      <c r="A88" s="90"/>
+      <c r="B88" s="93"/>
+      <c r="C88" s="95"/>
+      <c r="D88" s="97"/>
       <c r="E88" s="11">
         <v>815</v>
       </c>
@@ -5119,10 +4679,10 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="93"/>
-      <c r="B89" s="96"/>
-      <c r="C89" s="98"/>
-      <c r="D89" s="100"/>
+      <c r="A89" s="90"/>
+      <c r="B89" s="93"/>
+      <c r="C89" s="95"/>
+      <c r="D89" s="97"/>
       <c r="E89" s="11">
         <v>1723</v>
       </c>
@@ -5140,10 +4700,10 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="93"/>
-      <c r="B90" s="96"/>
-      <c r="C90" s="98"/>
-      <c r="D90" s="100"/>
+      <c r="A90" s="90"/>
+      <c r="B90" s="93"/>
+      <c r="C90" s="95"/>
+      <c r="D90" s="97"/>
       <c r="E90" s="11">
         <v>101</v>
       </c>
@@ -5161,10 +4721,10 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="93"/>
-      <c r="B91" s="96"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="101"/>
+      <c r="A91" s="90"/>
+      <c r="B91" s="93"/>
+      <c r="C91" s="95"/>
+      <c r="D91" s="98"/>
       <c r="E91" s="11">
         <v>1494</v>
       </c>
@@ -5182,29 +4742,29 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="93"/>
-      <c r="B92" s="96"/>
-      <c r="C92" s="98"/>
+      <c r="A92" s="90"/>
+      <c r="B92" s="93"/>
+      <c r="C92" s="95"/>
       <c r="D92" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="E92" s="102" t="s">
+      <c r="E92" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="F92" s="103"/>
-      <c r="G92" s="103"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="104"/>
+      <c r="F92" s="100"/>
+      <c r="G92" s="100"/>
+      <c r="H92" s="100"/>
+      <c r="I92" s="101"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="93"/>
+      <c r="A93" s="90"/>
       <c r="B93" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C93" s="105" t="s">
+      <c r="C93" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="D93" s="106"/>
+      <c r="D93" s="103"/>
       <c r="E93" s="33" t="s">
         <v>63</v>
       </c>
@@ -5214,103 +4774,103 @@
       <c r="G93" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H93" s="107"/>
-      <c r="I93" s="108"/>
+      <c r="H93" s="104"/>
+      <c r="I93" s="105"/>
     </row>
     <row r="94" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="93"/>
-      <c r="B94" s="43" t="s">
+      <c r="A94" s="90"/>
+      <c r="B94" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="76" t="s">
+      <c r="C94" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D94" s="77"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="79"/>
-      <c r="G94" s="46">
+      <c r="D94" s="74"/>
+      <c r="E94" s="75"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="43">
         <v>0.75239999999999996</v>
       </c>
-      <c r="H94" s="109"/>
-      <c r="I94" s="110"/>
+      <c r="H94" s="106"/>
+      <c r="I94" s="107"/>
     </row>
     <row r="95" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="93"/>
-      <c r="B95" s="47" t="s">
+      <c r="A95" s="90"/>
+      <c r="B95" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C95" s="80" t="s">
+      <c r="C95" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D95" s="81"/>
-      <c r="E95" s="81"/>
-      <c r="F95" s="82"/>
-      <c r="G95" s="48">
+      <c r="D95" s="78"/>
+      <c r="E95" s="78"/>
+      <c r="F95" s="79"/>
+      <c r="G95" s="45">
         <v>0.24759999999999999</v>
       </c>
-      <c r="H95" s="111"/>
-      <c r="I95" s="112"/>
+      <c r="H95" s="108"/>
+      <c r="I95" s="109"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="93"/>
-      <c r="B96" s="49" t="s">
+      <c r="A96" s="90"/>
+      <c r="B96" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C96" s="113" t="s">
+      <c r="C96" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D96" s="114"/>
-      <c r="E96" s="50" t="s">
+      <c r="D96" s="111"/>
+      <c r="E96" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F96" s="51">
+      <c r="F96" s="48">
         <v>0.28689999999999999</v>
       </c>
-      <c r="G96" s="51" t="s">
+      <c r="G96" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="H96" s="52" t="s">
+      <c r="H96" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="I96" s="74"/>
+      <c r="I96" s="71"/>
     </row>
     <row r="97" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="93"/>
+      <c r="A97" s="90"/>
       <c r="B97" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C97" s="76" t="s">
+      <c r="C97" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D97" s="77"/>
-      <c r="E97" s="78"/>
-      <c r="F97" s="79"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="76"/>
       <c r="G97" s="11">
         <v>0.83509999999999995</v>
       </c>
       <c r="H97" s="11">
         <v>0.1114</v>
       </c>
-      <c r="I97" s="74"/>
+      <c r="I97" s="71"/>
     </row>
     <row r="98" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="94"/>
+      <c r="A98" s="91"/>
       <c r="B98" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C98" s="80" t="s">
+      <c r="C98" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D98" s="81"/>
-      <c r="E98" s="81"/>
-      <c r="F98" s="82"/>
+      <c r="D98" s="78"/>
+      <c r="E98" s="78"/>
+      <c r="F98" s="79"/>
       <c r="G98" s="22">
         <v>0.16489999999999999</v>
       </c>
       <c r="H98" s="22">
         <v>0.1114</v>
       </c>
-      <c r="I98" s="75"/>
+      <c r="I98" s="72"/>
     </row>
     <row r="100" spans="1:9" ht="22" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
@@ -5319,17 +4879,17 @@
     </row>
     <row r="101" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="83" t="s">
+      <c r="A102" s="80" t="s">
         <v>129</v>
       </c>
       <c r="B102" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C102" s="86" t="s">
+      <c r="C102" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D102" s="87"/>
-      <c r="E102" s="53" t="s">
+      <c r="D102" s="84"/>
+      <c r="E102" s="50" t="s">
         <v>131</v>
       </c>
       <c r="F102" s="34">
@@ -5338,86 +4898,86 @@
       <c r="G102" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="H102" s="54" t="s">
+      <c r="H102" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="I102" s="88"/>
+      <c r="I102" s="85"/>
     </row>
     <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="84"/>
-      <c r="B103" s="43" t="s">
+      <c r="A103" s="81"/>
+      <c r="B103" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C103" s="76" t="s">
+      <c r="C103" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="D103" s="77"/>
-      <c r="E103" s="77"/>
-      <c r="F103" s="91"/>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
+      <c r="F103" s="88"/>
       <c r="G103" s="11">
         <v>0.83099999999999996</v>
       </c>
       <c r="H103" s="29">
         <v>3.04E-2</v>
       </c>
-      <c r="I103" s="89"/>
+      <c r="I103" s="86"/>
     </row>
     <row r="104" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="84"/>
-      <c r="B104" s="43" t="s">
+      <c r="A104" s="81"/>
+      <c r="B104" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C104" s="76" t="s">
+      <c r="C104" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D104" s="77"/>
-      <c r="E104" s="77"/>
-      <c r="F104" s="91"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="88"/>
       <c r="G104" s="11">
         <v>0.16900000000000001</v>
       </c>
       <c r="H104" s="29">
         <v>3.04E-2</v>
       </c>
-      <c r="I104" s="89"/>
+      <c r="I104" s="86"/>
     </row>
     <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="84"/>
-      <c r="B105" s="43" t="s">
+      <c r="A105" s="81"/>
+      <c r="B105" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C105" s="76" t="s">
+      <c r="C105" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="D105" s="77"/>
-      <c r="E105" s="77"/>
-      <c r="F105" s="91"/>
+      <c r="D105" s="74"/>
+      <c r="E105" s="74"/>
+      <c r="F105" s="88"/>
       <c r="G105" s="11">
         <v>0.78990000000000005</v>
       </c>
       <c r="H105" s="29">
         <v>0.1716</v>
       </c>
-      <c r="I105" s="89"/>
+      <c r="I105" s="86"/>
     </row>
     <row r="106" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="85"/>
-      <c r="B106" s="47" t="s">
+      <c r="A106" s="82"/>
+      <c r="B106" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C106" s="80" t="s">
+      <c r="C106" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D106" s="81"/>
-      <c r="E106" s="81"/>
-      <c r="F106" s="82"/>
+      <c r="D106" s="78"/>
+      <c r="E106" s="78"/>
+      <c r="F106" s="79"/>
       <c r="G106" s="22">
         <v>0.21010000000000001</v>
       </c>
-      <c r="H106" s="55">
+      <c r="H106" s="52">
         <v>0.1716</v>
       </c>
-      <c r="I106" s="90"/>
+      <c r="I106" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="97">

</xml_diff>